<commit_message>
m-ary tree card complete on LC
</commit_message>
<xml_diff>
--- a/DSA_pattern.xlsx
+++ b/DSA_pattern.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nitin_office_data\learning\DS_ALGO\DS_ALGO_PROG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B23B4E-FE93-45ED-87D4-37A347AC7050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946F2B0A-4551-42C5-BD8C-E5FA2A1D22CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94E546EF-B2FB-4067-B151-5AEC6D8CFD29}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>category</t>
   </si>
@@ -176,13 +176,80 @@
   </si>
   <si>
     <t>sliding window</t>
+  </si>
+  <si>
+    <t>Symmetric Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/data-structure-tree/17/solve-problems-recursively/536/</t>
+  </si>
+  <si>
+    <t>Iterative sol main logic is we can use queue and put right and left children of two nodes in opposite order i.e 
+  ```
+     q.offer(left.left);
+     q.offer(right.right);
+     q.offer(left.right);
+     q.offer(right.left);
+  ``` 
+recursive sol is intuitive i.e tree will be assymmetric if apposite children or left and right subtree do not match or if one is null and other is not</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/data-structure-tree/17/solve-problems-recursively/534/</t>
+  </si>
+  <si>
+    <t>recursion (top down / bottom up)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bottom up approach </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:  when problem can be divided into subprob and solved using sol of subprob then it's bottom up recursive approach it's similar to postorder traversal in tree first prob is solved for children and then using the ans from children main prob is solved.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Top-down"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> means that in each recursive call, we will visit the node first to come up with some values, and pass these values to its children when calling the function recursively. So the "top-down" solution can be considered as a kind of preorder traversal. </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +275,14 @@
       <sz val="8"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -560,10 +635,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D252FF50-3712-419C-915D-AA2F7E8133C5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +796,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -729,7 +804,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>40</v>
       </c>
@@ -737,7 +812,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>42</v>
       </c>
@@ -745,12 +820,34 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LC recursion backtracking WIP
</commit_message>
<xml_diff>
--- a/DSA_pattern.xlsx
+++ b/DSA_pattern.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nitin_office_data\learning\DS_ALGO\DS_ALGO_PROG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946F2B0A-4551-42C5-BD8C-E5FA2A1D22CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AAAFC3-3951-43DA-8E23-9B2CD2291A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94E546EF-B2FB-4067-B151-5AEC6D8CFD29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$22</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>category</t>
   </si>
@@ -244,12 +247,57 @@
       <t xml:space="preserve"> means that in each recursive call, we will visit the node first to come up with some values, and pass these values to its children when calling the function recursively. So the "top-down" solution can be considered as a kind of preorder traversal. </t>
     </r>
   </si>
+  <si>
+    <t>linkedlist</t>
+  </si>
+  <si>
+    <t>BST</t>
+  </si>
+  <si>
+    <t>heap</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>hashing</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t>Recursion</t>
+  </si>
+  <si>
+    <t>Swap Nodes in Pairs</t>
+  </si>
+  <si>
+    <t>recurse to last pair of node and then apply merging new head and next</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-i/250/principle-of-recursion/1681/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-i/250/principle-of-recursion/1681/discuss/2490014/simple-java-recursive-solution</t>
+  </si>
+  <si>
+    <t>my posts</t>
+  </si>
+  <si>
+    <t>time complexity calculation with recursion and memoization</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-i/256/complexity-analysis/1669/</t>
+  </si>
+  <si>
+    <t>no of recursive calls will not be always linear( chech fibonaacci recursive call tree is 2-ary tree in general it forms n-ary tree) but with memoization it can be made linear</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +332,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -306,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -319,6 +374,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -635,10 +691,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D252FF50-3712-419C-915D-AA2F7E8133C5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,7 +705,7 @@
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -662,8 +718,14 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -671,7 +733,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -682,7 +747,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -690,7 +758,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -698,7 +769,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -706,7 +780,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -714,7 +791,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -725,7 +805,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -736,7 +819,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -747,7 +833,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
       <c r="B11" t="s">
         <v>28</v>
       </c>
@@ -756,7 +845,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -764,7 +853,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
@@ -772,7 +864,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -780,7 +875,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -788,7 +886,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
       <c r="B16" t="s">
         <v>37</v>
       </c>
@@ -796,7 +897,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -804,7 +908,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
@@ -812,7 +919,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
       <c r="B19" t="s">
         <v>42</v>
       </c>
@@ -820,7 +930,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
       <c r="B20" t="s">
         <v>44</v>
       </c>
@@ -828,7 +941,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
       <c r="B21" t="s">
         <v>46</v>
       </c>
@@ -839,7 +955,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
       <c r="B22" t="s">
         <v>50</v>
       </c>
@@ -850,13 +969,46 @@
         <v>49</v>
       </c>
     </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:A22" xr:uid="{D252FF50-3712-419C-915D-AA2F7E8133C5}"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" location="to-detect-loop-and-find-first-node-of-the-loop-floyd-cycle-detetction-algorithm" tooltip="#to-detect-loop-and-find-first-node-of-the-loop-floyd-cycle-detetction-algorithm" display="vscode-resource://file/c%3A/nitin_office_data/learning/DS_ALGO/DS_ALGO_PROG/problem_with_pattern_and_solution.md - to-detect-loop-and-find-first-node-of-the-loop-floyd-cycle-detetction-algorithm" xr:uid="{B6E707AD-4420-489A-973D-89AE2A6DB0B5}"/>
     <hyperlink ref="D10" r:id="rId2" xr:uid="{6FEBE7B8-9C18-4D57-9A65-E935DD6E2680}"/>
+    <hyperlink ref="D23" r:id="rId3" xr:uid="{D9BD03ED-12E8-4FE0-9FB1-46BA6784414D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Helvetica 75 Bold"&amp;8&amp;KED7D31Orange Restricted</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
recursion / backtracking done LC
</commit_message>
<xml_diff>
--- a/DSA_pattern.xlsx
+++ b/DSA_pattern.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nitin_office_data\learning\DS_ALGO\DS_ALGO_PROG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AAAFC3-3951-43DA-8E23-9B2CD2291A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD94BD6-4CA6-4907-A3C6-20EC1A4B74FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94E546EF-B2FB-4067-B151-5AEC6D8CFD29}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="90">
   <si>
     <t>category</t>
   </si>
@@ -292,12 +292,82 @@
   <si>
     <t>no of recursive calls will not be always linear( chech fibonaacci recursive call tree is 2-ary tree in general it forms n-ary tree) but with memoization it can be made linear</t>
   </si>
+  <si>
+    <t>backtracking/Recursion</t>
+  </si>
+  <si>
+    <t>N-queen problem</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-ii/472/backtracking/2804/
+https://www.youtube.com/watch?v=i05Ju7AftcM</t>
+  </si>
+  <si>
+    <t>recursion and backtracking ( base check , loop through next candidates , check isSafe, place candidate, recurse for further down, backtrack i.e undo place candidate op)</t>
+  </si>
+  <si>
+    <t>generate parantheses</t>
+  </si>
+  <si>
+    <t>base cond is string length reaches 2*n and keep on adding ( when open count &lt; n and ) when count of close &lt; open</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/generate-parentheses/</t>
+  </si>
+  <si>
+    <t>sudoku solver</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-ii/472/backtracking/2796/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=FWAIf_EVUKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">using %, / for block traversal in matrix, 2 outer for loops for m*n board </t>
+  </si>
+  <si>
+    <t>leetcode 489 : robot room cleaner</t>
+  </si>
+  <si>
+    <t>https://zhenchaogan.gitbook.io/leetcode-solution/leetcode-489-robot-room-cleaner</t>
+  </si>
+  <si>
+    <t>robot can move in any 4 dir then come back to it's orignal pos for backtracking</t>
+  </si>
+  <si>
+    <t>combinations</t>
+  </si>
+  <si>
+    <t>take start, end in backtrack fn and use n-k+1 in for loop for perf improvement e.g for combine(4,2) no need to check for comb starting with 4 since it has been covered by those starting with 1,2,3</t>
+  </si>
+  <si>
+    <t>stack</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-ii/472/backtracking/2798/discuss/2580251/C29</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-ii/472/backtracking/2798/ </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-ii/507/beyond-recursion/2901/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=X0X6G-eWgQ8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">trick is to find the left smaller and right smaller for a bar at i that way max area for the bar is (rs -ls + 1) * bar height, to optimize compute the left &amp; right smaller array using stack </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +409,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -361,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -375,6 +451,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -691,10 +774,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D252FF50-3712-419C-915D-AA2F7E8133C5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -998,6 +1081,99 @@
       </c>
       <c r="D24" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
october challange 2 sum BST prob
</commit_message>
<xml_diff>
--- a/DSA_pattern.xlsx
+++ b/DSA_pattern.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nitin_office_data\learning\DS_ALGO\DS_ALGO_PROG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD94BD6-4CA6-4907-A3C6-20EC1A4B74FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644082D3-2365-45BC-8B7B-6147AAA431BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94E546EF-B2FB-4067-B151-5AEC6D8CFD29}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
   <si>
     <t>category</t>
   </si>
@@ -357,10 +357,31 @@
     <t>https://www.youtube.com/watch?v=X0X6G-eWgQ8</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">trick is to find the left smaller and right smaller for a bar at i that way max area for the bar is (rs -ls + 1) * bar height, to optimize compute the left &amp; right smaller array using stack </t>
+  </si>
+  <si>
+    <t>permutation</t>
+  </si>
+  <si>
+    <t>largest area in histogram</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-ii/507/beyond-recursion/2903/</t>
+  </si>
+  <si>
+    <t>general backtracking logic/ to improve TC use hashset/(boolean - preferred easy to explain &amp; understand) array or swapping logic</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-ii/507/beyond-recursion/2905/discuss/2606585/Easy-to-understand-clean-JAVA-backtracking-sol</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/recursion-ii/507/beyond-recursion/2905</t>
+  </si>
+  <si>
+    <t>Letter Combinations of a Phone Number</t>
+  </si>
+  <si>
+    <t>use backtracking and keypad map or an array / iterative sol uses queue FIFO</t>
   </si>
 </sst>
 </file>
@@ -774,10 +795,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D252FF50-3712-419C-915D-AA2F7E8133C5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,17 +1184,48 @@
       <c r="A30" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>86</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1182,9 +1234,10 @@
     <hyperlink ref="B3" r:id="rId1" location="to-detect-loop-and-find-first-node-of-the-loop-floyd-cycle-detetction-algorithm" tooltip="#to-detect-loop-and-find-first-node-of-the-loop-floyd-cycle-detetction-algorithm" display="vscode-resource://file/c%3A/nitin_office_data/learning/DS_ALGO/DS_ALGO_PROG/problem_with_pattern_and_solution.md - to-detect-loop-and-find-first-node-of-the-loop-floyd-cycle-detetction-algorithm" xr:uid="{B6E707AD-4420-489A-973D-89AE2A6DB0B5}"/>
     <hyperlink ref="D10" r:id="rId2" xr:uid="{6FEBE7B8-9C18-4D57-9A65-E935DD6E2680}"/>
     <hyperlink ref="D23" r:id="rId3" xr:uid="{D9BD03ED-12E8-4FE0-9FB1-46BA6784414D}"/>
+    <hyperlink ref="D32" r:id="rId4" xr:uid="{E0EAA414-E6FC-40E1-9A2C-894FA973F9D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Helvetica 75 Bold"&amp;8&amp;KED7D31Orange Restricted</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
sliding window + merge interval coding pattern + greedy pattern
</commit_message>
<xml_diff>
--- a/DSA_pattern.xlsx
+++ b/DSA_pattern.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nitin_office_data\learning\DS_ALGO\DS_ALGO_PROG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644082D3-2365-45BC-8B7B-6147AAA431BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268AD519-BD0C-4552-8D2A-56A553110D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94E546EF-B2FB-4067-B151-5AEC6D8CFD29}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{94E546EF-B2FB-4067-B151-5AEC6D8CFD29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="greedy" sheetId="4" r:id="rId2"/>
+    <sheet name="sliding window" sheetId="2" r:id="rId3"/>
+    <sheet name="merge-intervals" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
   <si>
     <t>category</t>
   </si>
@@ -383,12 +386,99 @@
   <si>
     <t>use backtracking and keypad map or an array / iterative sol uses queue FIFO</t>
   </si>
+  <si>
+    <t>1838. Frequency of the Most Frequent Element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sorting with sliding window </t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>209. Minimum Size Subarray Sum</t>
+  </si>
+  <si>
+    <t>sliding window 2 pointer</t>
+  </si>
+  <si>
+    <t>424. Longest Repeating Character Replacement</t>
+  </si>
+  <si>
+    <t>sliding window i.e invalid window condition is (curr window - most freq char count &gt; k) then we have to move left i.e shrink the window</t>
+  </si>
+  <si>
+    <t>Longest Substring with At Most K Distinct Characters</t>
+  </si>
+  <si>
+    <t>sliding window + map with char count to keep track of distinct curr in curr window so far</t>
+  </si>
+  <si>
+    <t>1004. Max Consecutive Ones III</t>
+  </si>
+  <si>
+    <t>sliding window + count of zeroes to shrink the window in case of invalid window size</t>
+  </si>
+  <si>
+    <t>56. Merge Intervals</t>
+  </si>
+  <si>
+    <t>greedy( sorting required ) + merge interval pattern</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/data-structure/merge-overlapping-sub-intervals/</t>
+  </si>
+  <si>
+    <t>57. Insert Interval</t>
+  </si>
+  <si>
+    <t>greedy( already sorting given) + merge interval pattern</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-interval/description/</t>
+  </si>
+  <si>
+    <t>N meetings in one room</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/data-structure/n-meetings-in-one-room/</t>
+  </si>
+  <si>
+    <t>986. Interval List Intersections</t>
+  </si>
+  <si>
+    <t>2 pointer with merge intervals pattern i.e overlapping conditions</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/interval-list-intersections/solutions/3984596/java-sol-with-explanation-2-pointers-with-merge-interval-patterns-overlapping-intervals/</t>
+  </si>
+  <si>
+    <t>435. Non-overlapping Intervals</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/non-overlapping-intervals/solutions/3984817/java-with-intuition-greedy-sorting-required-2-pointer-merge-overlapping-intervals-pattern/</t>
+  </si>
+  <si>
+    <t>greedy (sorting required) + 2 pointer with merge intervals pattern i.e overlapping conditions or we can count the max no of non-overlapping intervals and then len - max non overlapping gives min intervals to remove</t>
+  </si>
+  <si>
+    <t>Job Sequencing Problem</t>
+  </si>
+  <si>
+    <t>https://takeuforward.org/data-structure/job-sequencing-problem/</t>
+  </si>
+  <si>
+    <t>sorting based on profit and then checking is a job can be done on last day as per it's deadline so that meanwhile other jobs can done so take an array deadline with maxDeadline size and init with -1 then loop through the array and check if deadline can be done on last day i.e if deadlineArr[curr.deadline] == -1 then set it with job id and add profit job count etc else not check for prev free slot</t>
+  </si>
+  <si>
+    <t>greedy( already sorting given) + merge interval pattern create a Data structure with start, end , pos and apply sorting  and merge intervals pattern by simply checking lastAdded &lt; curr.start then curr becomes lastAdded assuming first meeting will always be included</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +526,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Titillium Web"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF090C10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -458,7 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -479,6 +581,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -797,8 +903,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1229,7 +1335,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A22" xr:uid="{D252FF50-3712-419C-915D-AA2F7E8133C5}"/>
+  <autoFilter ref="A1:A32" xr:uid="{D252FF50-3712-419C-915D-AA2F7E8133C5}"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" location="to-detect-loop-and-find-first-node-of-the-loop-floyd-cycle-detetction-algorithm" tooltip="#to-detect-loop-and-find-first-node-of-the-loop-floyd-cycle-detetction-algorithm" display="vscode-resource://file/c%3A/nitin_office_data/learning/DS_ALGO/DS_ALGO_PROG/problem_with_pattern_and_solution.md - to-detect-loop-and-find-first-node-of-the-loop-floyd-cycle-detetction-algorithm" xr:uid="{B6E707AD-4420-489A-973D-89AE2A6DB0B5}"/>
     <hyperlink ref="D10" r:id="rId2" xr:uid="{6FEBE7B8-9C18-4D57-9A65-E935DD6E2680}"/>
@@ -1242,4 +1348,277 @@
     <oddFooter>&amp;C&amp;1#&amp;"Helvetica 75 Bold"&amp;8&amp;KED7D31Orange Restricted</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC09495-4873-49FB-8D28-18497DAB9EB6}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="47.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925F63C8-0DB0-4E78-9EF8-A829194231E6}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://leetcode.com/problems/frequency-of-the-most-frequent-element/" xr:uid="{BE90D5D4-EFE9-47BF-B5F2-C328593B130F}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://leetcode.com/problems/minimum-size-subarray-sum/" xr:uid="{7C240BF9-5521-4061-8DC5-C7B7D3F47115}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://leetcode.com/problems/longest-repeating-character-replacement/" xr:uid="{1D097C35-2B9B-4293-B2C9-A70DA68FD297}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{72971011-6995-4DFC-BB5A-AFBA5756C2DA}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://leetcode.com/problems/max-consecutive-ones-iii/" xr:uid="{68131A94-16EA-4D5F-AEA5-A63216D1B3AC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DB69D5-E05E-4AC0-9830-00E57DD94D04}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="46.21875" customWidth="1"/>
+    <col min="3" max="3" width="53.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://leetcode.com/problems/merge-intervals/" xr:uid="{8AE0AFF5-F0D8-481C-8BE7-A539A9F55A88}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://leetcode.com/problems/insert-interval/" xr:uid="{7E97CA20-BEAE-48E3-A067-91B45946EB17}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://takeuforward.org/data-structure/n-meetings-in-one-room/" xr:uid="{8AA93C80-02AE-4E4D-87A8-B89F8EC3BDD7}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://leetcode.com/problems/interval-list-intersections/" xr:uid="{E18D2DE8-1C0D-499D-9BD7-367A199155CF}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://leetcode.com/problems/non-overlapping-intervals/" xr:uid="{AE29AB11-4F78-42E8-90FF-2A473578FF78}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{e6c818a6-e1a0-4a6e-a969-20d857c5dc62}" enabled="1" method="Standard" siteId="{90c7a20a-f34b-40bf-bc48-b9253b6f5d20}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>